<commit_message>
Added Code for Trapping Rain Water
</commit_message>
<xml_diff>
--- a/2.1. Two Pointers/5. Trapping Rain Water/good_test_cases.xlsx
+++ b/2.1. Two Pointers/5. Trapping Rain Water/good_test_cases.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Self-Study\LeetCode_Journey\2.1. Two Pointers\5. Trapping Rain Water\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28C609D-5C36-4A5A-AD59-CEB51960ED9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC907645-3864-4959-B700-A4FB73D31F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{CC0E9524-54F9-4FD0-A79B-ADADA3CA7E0D}"/>
+    <workbookView xWindow="0" yWindow="4275" windowWidth="21600" windowHeight="11325" xr2:uid="{CC0E9524-54F9-4FD0-A79B-ADADA3CA7E0D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Overtime" sheetId="1" r:id="rId1"/>
+    <sheet name="timeout" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -214,20 +214,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -592,18 +591,8 @@
         <v>0</v>
       </c>
       <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="8" t="s">
+      <c r="P1" s="2"/>
+      <c r="Q1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -615,428 +604,299 @@
         <v>6</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="3"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="3"/>
+      <c r="L3" s="4"/>
+      <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" s="1"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="17"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="16"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>0</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>2</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>3</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>4</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="7">
         <v>5</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="7">
         <v>6</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="7">
         <v>7</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="7">
         <v>8</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="7">
         <v>9</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <v>10</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="8" t="s">
+      <c r="P8" s="2"/>
+      <c r="Q8" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="3"/>
+      <c r="P9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="3"/>
+      <c r="L10" s="4"/>
+      <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E11" s="1"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="3"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="17"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="16"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>0</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>1</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>2</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>3</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>4</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="7">
         <v>5</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="7">
         <v>6</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="7">
         <v>7</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="7">
         <v>8</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="7">
         <v>9</v>
       </c>
-      <c r="O13" s="8">
+      <c r="O13" s="7">
         <v>10</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="8" t="s">
+      <c r="P15" s="2"/>
+      <c r="Q15" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="3"/>
+      <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E17" s="1"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="3"/>
+      <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="3"/>
+      <c r="L18" s="4"/>
+      <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="14"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="12"/>
     </row>
     <row r="20" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>0</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <v>1</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>2</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="7">
         <v>3</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="7">
         <v>4</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="7">
         <v>5</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="7">
         <v>6</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L20" s="7">
         <v>7</v>
       </c>
-      <c r="M20" s="8">
+      <c r="M20" s="7">
         <v>8</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N20" s="7">
         <v>9</v>
       </c>
-      <c r="O20" s="8">
+      <c r="O20" s="7">
         <v>10</v>
       </c>
-      <c r="P20" s="8">
+      <c r="P20" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E22" s="1"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="8" t="s">
+      <c r="P22" s="2"/>
+      <c r="Q22" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E23" s="1"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="3"/>
+      <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E24" s="1"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="3"/>
+      <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E25" s="1"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="3"/>
+      <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="14"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="12"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E27" s="8">
+      <c r="E27" s="7">
         <v>0</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="7">
         <v>1</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="7">
         <v>2</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="7">
         <v>3</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I27" s="7">
         <v>4</v>
       </c>
-      <c r="J27" s="8">
+      <c r="J27" s="7">
         <v>5</v>
       </c>
-      <c r="K27" s="8">
+      <c r="K27" s="7">
         <v>6</v>
       </c>
-      <c r="L27" s="8">
+      <c r="L27" s="7">
         <v>7</v>
       </c>
-      <c r="M27" s="8">
+      <c r="M27" s="7">
         <v>8</v>
       </c>
-      <c r="N27" s="8">
+      <c r="N27" s="7">
         <v>9</v>
       </c>
-      <c r="O27" s="8">
+      <c r="O27" s="7">
         <v>10</v>
       </c>
-      <c r="P27" s="8">
+      <c r="P27" s="7">
         <v>11</v>
       </c>
     </row>
@@ -1048,12 +908,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3"/>
-      <c r="P29" s="2"/>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1063,61 +918,57 @@
         <v>9</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="6"/>
+      <c r="J30" s="5"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E31" s="11"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="6"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E32" s="11"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="6"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="5"/>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E33" s="11"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="6"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="5"/>
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E34" s="12"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="7"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="6"/>
     </row>
     <row r="35" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E35" s="8">
+      <c r="E35" s="7">
         <v>0</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="7">
         <v>1</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="7">
         <v>2</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="7">
         <v>3</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I35" s="7">
         <v>4</v>
       </c>
-      <c r="J35" s="8">
+      <c r="J35" s="7">
         <v>5</v>
       </c>
     </row>

</xml_diff>